<commit_message>
automatic html creation improvements and dk and pt added to some products
</commit_message>
<xml_diff>
--- a/ePICreator/data/Humalog.xlsx
+++ b/ePICreator/data/Humalog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoalmeida/Desktop/hl7Europe/gravitate/gravitate-health/ePICreator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoalmeida/Desktop/hl7Europe/gravitate/gravitate-health/ePICreator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382F42F0-BFAC-8343-90A4-C53CD338719B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794121DF-8DBF-B446-ADF7-229CBB121CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" firstSheet="1" activeTab="10" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" firstSheet="1" activeTab="10" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
   </bookViews>
   <sheets>
     <sheet name="AdministrableProductDefinition" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="182">
   <si>
     <t>id</t>
   </si>
@@ -1130,6 +1130,563 @@
   </si>
   <si>
     <t>humalog-id</t>
+  </si>
+  <si>
+    <t>dk</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;B. INDLÆGSSEDDEL 
+Indlægsseddel: Information til brugeren &lt;/p&gt;
+&lt;p&gt;Humalog 100 enheder/ml injektionsvæske, opløsning, i hætteglas 
+insulin lispro &lt;/p&gt;
+&lt;p&gt;Læs denne indlægsseddel grundigt, inden du begynder at bruge dette lægemiddel, da den 
+indeholder vigtige oplysninger. 
+- Gem indlægssedlen. Du kan få brug for at læse den igen. 
+- Spørg lægen eller apotekspersonalet, hvis der er mere, du vil vide. 
+- Lægen har ordineret dette lægemiddel til dig personligt. Lad derfor være med at give medicinen 
+til andre. Det kan være skadeligt for andre, selvom de har de samme symptomer, som du har. 
+- Kontakt lægen eller apotekspersonalet, hvis du får bivirkninger, herunder bivirkninger, som ikke 
+er nævnt i denne indlægsseddel. Se punkt 4.&lt;br /&gt;
+Se den nyeste indlægsseddel på www.indlaegsseddel.dk. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Oversigt over indlægssedlen 
+1. Virkning og anvendelse 
+2. Det skal du vide, før du begynder at bruge Humalog 
+3. Sådan skal du bruge Humalog 
+4. Bivirkninger&lt;br /&gt;
+5. Opbevaring 
+6. Pakningsstørrelser og yderligere oplysninger &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Humalog anvendes til at behandle diabetes. Humalog virker hurtigere end almindelig human insulin, 
+fordi insulinmolekylet er blevet ændret en smule. &lt;/p&gt;
+&lt;p&gt;Du får diabetes, hvis din bugspytkirtel ikke producerer tilstrækkeligt insulin til at kontrollere dit 
+blodsukkerniveau. Humalog er en erstatning for dit eget insulin og bruges til at kontrollere dit 
+blodsukker på langt sigt. Det virker meget hurtigt og i kortere tid end opløselig insulin (2 til 5 timer). 
+Du bør normalt anvende Humalog indenfor 15 minutter før eller efter et måltid. &lt;/p&gt;
+&lt;p&gt;Din læge kan bede dig om at bruge Humalog sammen med et længerevirkende insulin. Til hver 
+insulintype hører en separat indlægsseddel med oplysninger om den enkelte insulintype. Du må ikke 
+ændre din insulinbehandling, medmindre din læge beder dig om det. Vær meget forsigtig, hvis du skal 
+ændre insulin. &lt;/p&gt;
+&lt;p&gt;Humalog kan bruges af voksne og børn. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Brug IKKE Humalog 
+- hvis du føler, at du er ved at få hypoglykæmi (lavt blodsukker). Senere i denne indlægsseddel 
+beskrives, hvordan du skal behandle et let tilfælde af hypoglykæmi (se punkt 3: Hvis du har 
+taget for meget Humalog). 
+- hvis du er allergisk over for insulin lispro eller et af de øvrige indholdsstoffer i Humalog 
+(angivet i punkt 6). &lt;/p&gt;
+&lt;p&gt;Advarsler og forsigtighedsregler &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;
+&lt;p&gt;Kontrollér altid insulinets navn og type på æsken og hætteglassets etiket, når du får insulinet fra 
+apoteket. Vær opmærksom på, at du får det Humalog, som din læge har sagt, at du skal bruge. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Hvis dit blodsukkerniveau er velkontrolleret med din nuværende insulinbehandling, fornemmer 
+du måske ikke advarselssymptomerne, når dit blodsukker bliver for lavt. Advarselssymptomer 
+beskrives senere i denne indlægsseddel. Du må derfor grundigt overveje, hvornår du vil lægge 
+dine måltider, hvor ofte du vil dyrke motion og hvor meget. Du skal også holde nøje øje med dit 
+blodsukkerniveau ved ofte at måle dit blodsukker. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Enkelte personer, som har haft hypoglykæmi efter at have skiftet fra animalsk insulin til human 
+insulin har fortalt, at de tidlige advarselssymptomer for human insulin var mindre tydelige eller 
+forskellige fra animalsk insulin. Hvis du ofte har hypoglykæmi eller har svært ved at føle det, 
+bør du tale med din læge om det. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Hvis du kan svare JA til et hvilket som helst af nedenstående spørgsmål, skal du fortælle det til 
+din læge, diabetessygeplejerske eller på dit apotek. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;Har du været syg for nylig? &lt;/li&gt;
+&lt;li&gt;Har du symptomer fra dine nyrer eller lever? &lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Dyrker du mere motion end normalt? &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Dit insulinbehov kan også ændres, hvis du indtager alkohol. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Du skal også fortælle din læge, diabetessygeplejerske eller dit apotek, hvis du planlægger at 
+rejse til udlandet. Tidsforskellen mellem lande kan betyde, at du skal have dine injektioner og 
+måltider på andre tidspunkter, end når du er hjemme. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Nogle patienter med årelang type 2-diabetes mellitus og hjertesygdom eller tidligere 
+slagtilfælde, og som blev behandlet med pioglitazon og insulin, udviklede hjertesvigt. Fortæl det 
+til din læge hurtigst muligt, hvis du oplever tegn på hjertesvigt, f.eks. hvis du bliver usædvanligt 
+stakåndet eller får hurtig vægtstigning eller væskeansamlinger (ødemer). &lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Hudforandringer på injektionsstedet 
+Injektionsstedet bør løbende skiftes for at forebygge hudforandringer, f.eks. knuder under huden. Hvis 
+du injicerer insulinet i et område med knuder, kan det være, at insulinet ikke virker så godt (se afsnittet 
+Sådan skal du bruge Humalog). Kontakt lægen, hvis du for øjeblikket injicerer i et område med 
+knuder, før du begynder at injicere i et andet område. Det kan være, at lægen vil fortælle dig, at du 
+skal tjekke dit blodsukker oftere og tilpasse insulindosen eller dosen af andre antidiabetiske 
+lægemidler. &lt;/p&gt;
+&lt;p&gt;Brug af anden medicin sammen med Humalog 
+Dit insulinbehov kan ændre sig hvis du tager: &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;
+&lt;p&gt;p-piller, &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;steroider, &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;skjoldbruskkirtelhormon, &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;orale antidiabetika, &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;acetylsalicylsyre, &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;sulfapræparater, &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;octreotid, &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;beta2-stimulerende midler (f.eks. ritodrin, salbutamol eller terbutalin), &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;beta-blokkere, &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;visse midler mod depression (monoaminooxidasehæmmere eller selektive 
+serotoningenoptagshæmmere (SSRI)), &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;danazol, &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;visse ACE-hæmmere (f.eks. captopril og enalapril) og &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;angiotensin II-receptorblokkere. &lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Fortæl det altid til lægen eller apotekspersonalet, hvis du bruger anden medicin, for nylig har brugt 
+anden medicin eller planlægger at bruge anden medicin. Dette gælder også medicin, som ikke er købt 
+på recept (se punkt ”Advarsler og forsigtighedsregler”). &lt;/p&gt;
+&lt;p&gt;Graviditet og amning 
+Hvis du er gravid eller ammer, har mistanke om, at du er gravid, eller planlægger at blive gravid, skal 
+du spørge din læge eller apotekspersonalet til råds, før du tager dette lægemiddel. &lt;/p&gt;
+&lt;p&gt;Dit insulinbehov vil sædvanligvis nedsættes under de første 3 måneder af graviditeten og øges under 
+de resterende 6 måneder af graviditeten. Hvis du ammer, kan det være nødvendigt at justere din 
+insulindosis eller din kost. &lt;/p&gt;
+&lt;p&gt;Trafik- og arbejdssikkerhed 
+Din koncentrations- og reaktionsevne kan være nedsat, hvis du har hypoglykæmi (lavt blodsukker). 
+Vær opmærksom på dette i alle situationer, hvor du kan bringe dig selv eller andre i fare (f.eks. ved 
+bilkørsel eller ved betjening af maskiner). Du bør drøfte med din læge om bilkørsel er tilrådeligt, hvis 
+du har: &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;
+&lt;p&gt;hyppige tilfælde af hypoglykæmi &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;nedsat eller manglende evne til at mærke advarselstegn på hypoglykæmi &lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Humalog indeholder natrium 
+Dette lægemiddel indeholder mindre end 1 mmol (23 mg) natrium pr. dosis, dvs. det er i det 
+væsentlige natriumfrit. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Brug altid lægemidlet nøjagtigt efter lægens anvisning. Er du i tvivl, så spørg lægen eller 
+apotekspersonalet. &lt;/p&gt;
+&lt;p&gt;Dosis &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;
+&lt;p&gt;Du bør normalt injicere Humalog indenfor 15 minutter før et måltid. Hvis det er nødvendigt, kan 
+du injicere Humalog lige efter et måltid. Din læge har fortalt dig præcist, hvor meget du skal 
+bruge, hvornår du skal bruge det og hvor ofte. Lægens instruktioner gælder kun for dig. Følg 
+dem nøjagtigt og besøg dit diabetesambulatorium regelmæssigt. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Hvis du ændrer insulintype (f.eks. fra human eller animalsk insulin til et Humalog produkt), skal 
+du måske tage mere eller mindre insulin end før. Dette gælder måske kun den første injektion 
+eller kan være en gradvis ændring over flere uger eller måneder. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Injicer Humalog under huden. Du bør kun injicere Humalog i en muskel, hvis din læge har sagt 
+dette. &lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Klargøring af Humalog &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Humalog er allerede opløst i vand, så du behøver ikke at blande det. Du må dog kun bruge 
+opløsningen, hvis den ser ud som vand. Den skal være klar, farveløs og uden faste partikler. 
+Kontrollér dette før hver injektion. &lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Injektion af Humalog &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;
+&lt;p&gt;Vask hænderne. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Rens huden som anvist før du foretager en injektion. Rens gummimembranen på hætteglasset, 
+men fjern den ikke. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Brug en ren, steril sprøjte og kanyle til at stikke gennem gummimembranen og træk den 
+ønskede dosis Humalog op i sprøjten. Din læge eller dit diabetesambulatorium vil fortælle dig, 
+hvordan du skal gøre dette. Del ikke dine kanyler og sprøjter med andre. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Injicer Humalog under huden, som du er blevet instrueret. Injicer ikke direkte i en blodåre. Efter 
+injektionen skal du lade kanylen blive i huden i 5 sekunder for at være sikker på, at du har fået 
+hele din dosis. Gnid ikke på indstiksstedet. Vær opmærksom på, at injicere mindst 1 cm fra 
+forrige indstikssted og at skifte indstikssted mellem hver injektion, som du er blevet instrueret. 
+Uanset om du injicerer i overarmen, låret, balden eller maven, virker din Humalog injektion 
+hurtigere end almindelg insulin. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Din læge vil fortælle dig, hvis du skal blande Humalog med en af de humane insuliner. Hvis du 
+skal injicere en blanding, skal Humalog trækkes op i sprøjten før det længerevirkende insulin. 
+Injicer væsken umiddelbart efter, at du har blandet den. Gør på samme måde hver gang. Du bør 
+almindeligvis ikke blande Humalog med blandinger af human insulin. Du bør aldrig blande 
+Humalog med insulinpræparater fremstillet af andre producenter eller med animalsk insulin. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Du må ikke injicere Humalog direkte i blodet. Injicer Humalog som din læge eller 
+diabetessygeplejerske har lært dig. Det er kun din læge der kan give dig Humalog direkte i 
+blodet. Lægen kan benytte sig af denne mulighed i ganske særlige tilfælde, f.eks. under en 
+operation eller hvis dit blodsukker bliver for højt under en sygdom. &lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Brug af Humalog i en infusionspumpe &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;
+&lt;p&gt;Kun visse CE-mærkede insulininfusionspumper kan anvendes til infusion af insulin lispro. Før 
+infusion af insulin lispro påbegyndes skal fremstillerens instruktioner læses igennem for at sikre 
+egnetheden samt andet i relation til den pågældende pumpe. Læs og følg instruktionerne i 
+produktinformationen, der følger med infusionspumpen. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Vær sikker på, at du bruger det rigtige reservoir og infusionskateter til din pumpe. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Skift af infusionssættet (slange og kanyle) skal ske i overensstemmelse med de instruktioner, 
+som er i brugsanvisningen, der følger med infusionssættet. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;I tilfælde af hypoglykæmi bør infusionen stoppes, indtil det hypoglykæmiske tilfælde er 
+overstået. Hvis der forekommer gentagne eller svært nedsatte blodsukkerniveauer, bør du 
+informere din læge eller dit diabetesambulatorium, og du bør overveje, om det er nødvendigt at 
+nedsætte eller stoppe din insulininfusion. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;En fejl ved pumpen eller tilstopning af infusionssættet kan give en hurtig stigning af 
+blodsukkerniveauet. Hvis du har mistanke om, at insulinflowet er afbrudt, bør du følge 
+instruktionerne i produktinformationen og hvis nødvendigt informere din læge eller dit 
+diabetesambulatorium. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Når Humalog bruges i en insulininfusionspumpe, bør det ikke blandes med andet insulin. &lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Hvis du har taget for meget Humalog 
+Hvis du tager mere Humalog end du bør eller er usikker på, hvor meget du har injiceret, kan det ske, at 
+dit blodsukker bliver for lavt. Kontrollér dit blodsukker.  &lt;/p&gt;
+&lt;p&gt;Hvis dit blodsukker er lavt (let hypoglykæmi), skal du spise druesukker, sukker eller drikke en 
+sukkerholdig drik. Derefter bør du spise frugt, kiks eller brød efter din læges råd og hvile dig. Dette vil 
+ofte hjælpe dig over et let tilfælde af hypoglykæmi eller en mindre insulinoverdosis. Hvis du får det 
+værre, din vejrtrækning bliver overfladisk og din hud bleg, skal du straks informere din læge. En 
+injektion med glukagon kan behandle selv svær hypoglykæmi. Indtag druesukker eller sukker efter 
+glukagon-injektionen. Hvis du ikke reagerer på glukagon, skal du på hospitalet. Bed din læge fortælle 
+dig om glukagon. &lt;/p&gt;
+&lt;p&gt;Hvis du har glemt at tage Humalog&lt;br /&gt;
+Hvis du glemmer at tage Humalog eller er usikker på, hvor meget du har injiceret, kan det ske, at dit 
+blodsukker bliver for højt. Kontrollér dit blodsukker. &lt;/p&gt;
+&lt;p&gt;Hvis hypoglykæmi (lavt blodsukker) eller hyperglykæmi (højt blodsukker) ikke bliver behandlet, kan 
+disse tilstande blive meget alvorlige og forårsage hovedpine, kvalme, opkastning, dehydrering, 
+bevidstløshed, koma og i værste fald medføre døden (se afsnit A og B under punkt 4 ”Bivirkninger”). &lt;/p&gt;
+&lt;p&gt;De tre enkle trin til at undgå hypoglykæmi eller hyperglykæmi er:  &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;
+&lt;p&gt;Opbevar altid ekstra éngangssprøjter og et ekstra Humalog hætteglas. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Medbring altid noget, der viser, at du er diabetiker. &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;Hav altid sukker på dig. &lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Hvis du holder op med at tage Humalog 
+Hvis du holder op med at tage Humalog, kan det ske, at dit blodsukker bliver for højt. Du må ikke 
+ændre din insulinbehandling, medmindre din læge beder dig om det. &lt;/p&gt;
+&lt;p&gt;Spørg lægen eller apotekspersonalet, hvis der er noget, du er i tvivl om. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Dette lægemiddel kan som alle andre lægemidler give bivirkninger, men ikke alle får bivirkninger. &lt;/p&gt;
+&lt;p&gt;Systemisk allergi er sjælden (≥ 1/10.000 til &amp;lt;1/1.000). Symptomerne er: &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;
+&lt;p&gt;udslæt over hele kroppen   &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;faldende blodtryk &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;vejrtrækningsbesvær &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;hjertebanken &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;hvæsende vejrtrækning &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;svedtendens 
+Hvis du tror, at du har denne form for insulinallergi med Humalog, skal du straks informere din læge. &lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Lokal allergi er almindelig (≥ 1/100 til &amp;lt;1/10). Nogle mennesker får rødme, hævelse eller kløe 
+omkring indstiksstedet. Dette forsvinder sædvanligvis i løbet af få dage til få uger. Informér din læge, 
+hvis du oplever dette. &lt;/p&gt;
+&lt;p&gt;Lipodystrofi er ikke almindelig (≥ 1/1.000 til &amp;lt;1/100). Hvis du injicerer insulin for ofte på samme 
+sted, kan fedtvævet enten skrumpe (lipoartrofi) eller fortykkes (lipohypertrofi). Knuder under huden 
+kan også skyldes ophobning af et protein, der kaldes amyloid (kutan amyloidose). Hvis du injicerer 
+insulinet i et område med knuder, kan det være, at insulinet ikke virker så godt. Skift injektionssted 
+ved hver injektion for at forebygge disse hudforandringer. &lt;/p&gt;
+&lt;p&gt;Væskeophobning (ødem, f.eks hævelse af armene, anklerne) er blevet indberettet, specielt i starten af 
+insulinbehandlingen, eller hvis behandlingen ændres for at forbedre kontrollen med dit blodsukker. &lt;/p&gt;
+&lt;p&gt;Indberetning af bivirkninger 
+Hvis du oplever bivirkninger, bør du tale med din læge eller apotekspersonalet. Dette gælder også 
+mulige bivirkninger, som ikke er medtaget i denne indlægsseddel. Du eller dine pårørende kan også 
+indberette bivirkninger direkte til Lægemiddelstyrelsen via det nationale rapporteringssystem anført i 
+Appendiks V. Ved at indrapportere bivirkninger kan du hjælpe med at fremskaffe mere information 
+om sikkerheden af dette lægemiddel. &lt;/p&gt;
+&lt;p&gt;Almindelige problemer ved diabetes &lt;/p&gt;
+&lt;p&gt;A.&lt;br /&gt;
+Hypoglykæmi 
+Hypoglykæmi (lavt blodsukker) betyder, at der ikke er tilstrækkeligt sukker i blodet. Dette kan 
+skyldes, at: &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;
+&lt;p&gt;du tager for meget Humalog eller andet insulin; &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;du springer et måltid over, det bliver forsinket, eller at du ændrer din kost; &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;du motionerer eller arbejder for hårdt lige før eller efter et måltid; &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;du har en infektion, eller du er syg (specielt diarré eller opkastning); &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;der er en ændring i dit behov for insulin; eller &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;du har nyre- eller leverproblemer, der forværres. &lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Alkohol og visse lægemidler kan påvirke dit blodsukkerniveau. &lt;/p&gt;
+&lt;p&gt;De første symptomer på for lavt blodsukker kommer sædvanligvis hurtigt og inkluderer: &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;
+&lt;p&gt;træthed  &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;hjertebanken &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;nervøsitet eller kulderystelser &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;kvalme &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;hovedpine &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;koldsved &lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Hvis du ikke er sikker på advarselssymptomerne på hypoglykæmi, bør du undgå situationer, som f.eks. 
+bilkørsel, hvor du selv eller andre kan komme i fare på grund af hypoglykæmi. &lt;/p&gt;
+&lt;p&gt;B.&lt;br /&gt;
+Hyperglykæmi og diabetisk ketoacidose (syreforgiftning) 
+Hyperglykæmi (højt blodsukker) betyder, at din krop ikke har tilstrækkeligt insulin. Hyperglykæmi 
+kan være forårsaget af: &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;
+&lt;p&gt;at du ikke tager Humalog eller andet insulin; &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;at du tager mindre insulin, end din læge har anvist; &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;at du spiser mere, end din diæt tillader dig; eller &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;feber, infektion eller følelsesmæssig ubalance. &lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Hyperglykæmi kan resultere i diabetisk ketoacidose. De første symptomer kommer langsomt over 
+mange timer eller dage. Symptomerne inkluderer følgende: &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;
+&lt;p&gt;træthed &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;manglende appetit &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;blussende ansigt &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;frugtagtig ånde &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;tørst  &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;
+&lt;p&gt;kvalme og opkastning &lt;/p&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Svære symptomer er tung vejrtrækning og hurtig puls. Søg lægehjælp straks. &lt;/p&gt;
+&lt;p&gt;C.&lt;br /&gt;
+Sygdom 
+Hvis du er syg, særligt hvis du har kvalme eller opkastning, kan dit insulinbehov ændre sig. Selv når 
+du ikke spiser normalt, har du stadig brug for insulin. Test din urin eller dit blod, følg de 
+almindelige regler ved sygdom og informér din læge. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Humalog opbevares i køleskab (2ºC – 8ºC), indtil det tages i brug for første gang. Må ikke nedfryses. 
+Det hætteglas, der er i brug, opbevares i et køleskab (2ºC – 8ºC) eller ved stuetemperatur (under 30ºC) 
+og kasseres efter 28 dage. Læg det ikke nær varme eller i solen. &lt;/p&gt;
+&lt;p&gt;Opbevar lægemidlet utilgængeligt for børn. &lt;/p&gt;
+&lt;p&gt;Brug ikke lægemidlet efter den udløbsdato, der står på etiketten og æsken efter EXP. Udløbsdatoen er 
+den sidste dag i den nævnte måned. &lt;/p&gt;
+&lt;p&gt;Brug ikke lægemidlet, hvis du ser en farvning af produktet, eller hvis der er faste partikler i produktet. 
+Du må kun bruge det, hvis det ser ud som vand. Kontrollér det hver gang du skal injicere dig selv. &lt;/p&gt;
+&lt;p&gt;Spørg apotekspersonalet, hvordan du skal bortskaffe medicinrester. Af hensyn til miljøet må du ikke 
+smide medicinrester i afløbet, toilettet eller skraldespanden. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Humalog 100 enheder/ml injektionsvæske, opløsning, i hætteglas indeholder: 
+- Aktivt stof: insulin lispro. Insulin lispro er fremstillet ved gensplejsning. Det er en ændret form 
+for human insulin og er derfor forskellig fra andre humane og animalske insuliner. Insulin lispro 
+er nært beslægtet med human insulin, som er et naturligt hormon, der produceres af kroppens 
+bugspytkirtel. 
+- Øvrige indholdsstoffer: m-cresol, glycerol, dinatriumphosphat heptahydrat, zinkoxid og vand til 
+injektionsvæsker. Natriumhydroxid eller saltsyre kan være tilsat for at justere surhedsgraden 
+(pH). &lt;/p&gt;
+&lt;p&gt;Udseende og pakningsstørrelser 
+Humalog 100 enheder/ml injektionsvæske, opløsning er en steril klar farveløs vandig opløsning og 
+indeholder 100 enheder insulin lispro per milliliter (100 enheder/ml) injektionsvæske. Hvert hætteglas 
+indeholder 1000 enheder (10 milliliter). Humalog 100 enheder/ml injektionsvæske, opløsning, i 
+hætteglas findes i pakninger med 1 hætteglas, 2 hætteglas samt i en multipakning med 5 x 1 hætteglas. 
+Ikke alle pakningsstørrelser er nødvendigvis markedsført. &lt;/p&gt;
+&lt;p&gt;Indehaver af markedsføringstilladelsen og fremstiller 
+Humalog 100 enheder/ml injektionsvæske, opløsning, i hætteglas fremstilles af: &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Lilly S.A., Avda. de la Industria 30, 28108 Alcobendas, Madrid, Spanien. &lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Indehaver af markedsføringstilladelsen er: Eli Lilly Nederland B.V., Papendorpseweg 83, 3528 BJ 
+Utrecht, Holland. &lt;/p&gt;
+&lt;p&gt;Hvis du ønsker yderligere oplysninger om dette lægemiddel, skal du henvende dig til den lokale 
+repræsentant for indehaveren af markedsføringstilladelsen: &lt;/p&gt;
+&lt;p&gt;Belgique/België/Belgien 
+Eli Lilly Benelux S.A./N.V. 
+Tél/Tel: + 32-(0)2 548 84 Lietuva 
+Eli Lilly Lietuva 
+Tel. +370 (5) 2649 
+България 
+ТП "Ели Лили Недерланд" Б.В. - България 
+тел. + 359 2 491 41 Luxembourg/Luxemburg 
+Eli Lilly Benelux S.A./N.V. 
+Tél/Tel: + 32-(0)2 548 84&lt;br /&gt;
+Česká republika 
+ELI LILLY ČR, s.r.o. 
+Tel: + 420 234 664 Magyarország 
+Lilly Hungária Kft. 
+Tel: + 36 1 328 5 
+Danmark 
+Eli Lilly Danmark A/S&lt;br /&gt;
+Tlf: +45 45 26 6Malta 
+Charles de Giorgio Ltd. 
+Tel: + 356 25600&lt;br /&gt;
+Deutschland 
+Lilly Deutschland GmbH 
+Tel. + 49-(0) 6172 273 2Nederland 
+Eli Lilly Nederland B.V.&lt;br /&gt;
+Tel: + 31-(0) 30 60 25&lt;br /&gt;
+Eesti 
+Eli Lilly Nederland B.V.&lt;br /&gt;
+Tel: +372 6817 Norge 
+Eli Lilly Norge A.S.&lt;br /&gt;
+Tlf: + 47 22 88 18&lt;br /&gt;
+Ελλάδα 
+ΦΑΡΜΑΣΕΡΒ-ΛΙΛΛΥ Α.Ε.Β.Ε.&lt;br /&gt;
+Τηλ: +30 210 629 4Österreich 
+Eli Lilly Ges. m.b.H.&lt;br /&gt;
+Tel: + 43-(0) 1 711&lt;br /&gt;
+España 
+Lilly S.A. 
+Tel: + 34-91 663 50 Polska 
+Eli Lilly Polska Sp. z o.o. 
+Tel: +48 22 440 33&lt;br /&gt;
+France 
+Lilly France 
+Tél: +33-(0) 1 55 49 34 Portugal 
+Lilly Portugal - Produtos Farmacêuticos, Lda 
+Tel: + 351-21-4126 
+Hrvatska 
+Eli Lilly Hrvatska d.o.o. 
+Tel: +385 1 2350 România 
+Eli Lilly România S.R.L. 
+Tel: + 40 21 4023 
+Ireland 
+Eli Lilly and Company (Ireland) Limited 
+Tel: + 353-(0) 1 661 4Slovenija 
+Eli Lilly farmacevtska družba, d.o.o. 
+Tel: +386 (0) 1 580 00&lt;br /&gt;
+Ísland 
+Icepharma hf.&lt;br /&gt;
+Sími + 354 540 8Slovenská republika 
+Eli Lilly Slovakia s.r.o. 
+Tel: + 421 220 663&lt;br /&gt;
+Italia 
+Eli Lilly Italia S.p.A. 
+Suomi/Finland 
+Oy Eli Lilly Finland Ab&lt;br /&gt;
+Tel: + 39- 055 42Puh/Tel: + 358-(0) 9 85 45&lt;br /&gt;
+Κύπρος 
+Phadisco Ltd&lt;br /&gt;
+Τηλ: +357 22 715Sverige 
+Eli Lilly Sweden AB 
+Tel: + 46-(0) 8 7378 
+Latvija 
+Eli Lilly (Suisse) S.A Pārstāvniecība Latvijā 
+Tel: +371 67364United Kingdom (Northern Ireland) 
+Eli Lilly and Company (Ireland) Limited 
+Tel: + 353-(0) 1 661 4377  &lt;/p&gt;
+&lt;p&gt;Denne indlægsseddel blev senest ændret {MM/ÅÅÅÅ} &lt;/p&gt;
+&lt;p&gt;Du kan finde yderligere oplysninger om dette lægemiddel på Det Europæiske Lægemiddelagenturs 
+hjemmeside http://www.ema.europa.eu&lt;br /&gt;
+Indlægsseddel: Information til brugeren &lt;/p&gt;
+&lt;p&gt;Humalog 100 enheder/ml injektionsvæske, opløsning, i cylinderampul&lt;br /&gt;
+insulin lispro &lt;/p&gt;
+&lt;p&gt;Læs denne indlægsseddel grundigt, inden du begynder at bruge dette lægemiddel, da den 
+indeholder vigtige oplysninger. 
+- Gem indlægssedlen. Du kan få brug for at læse den igen. 
+- Spørg lægen eller apotekspersonalet, hvis der er mere, du vil vide. 
+- Lægen har ordineret dette lægemiddel til dig personligt. Lad derfor være med at give medicinen 
+til andre. Det kan være skadeligt for andre, selvom de har de samme symptomer, som du har. 
+- Kontakt lægen eller apotekspersonalet, hvis du får bivirkninger, herunder bivirkninger, som ikke 
+er nævnt i denne indlægsseddel. Se punkt 4.&lt;br /&gt;
+Se den nyeste indlægsseddel på www.indlaegsseddel.dk. &lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -1313,9 +1870,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1353,7 +1910,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1459,7 +2016,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1601,7 +2158,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1810,10 +2367,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB4B3880-CBCE-B242-93DB-BF401DA7FB8A}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1855,8 +2412,23 @@
         <v>26</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" t="s">
+        <v>173</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1923,10 +2495,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05DE958-7C5A-B14B-9983-3CEB258B5640}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2029,8 +2601,48 @@
         <v>170</v>
       </c>
     </row>
+    <row r="3" spans="1:16" ht="409.6">
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updates correction language code
</commit_message>
<xml_diff>
--- a/ePICreator/data/Humalog.xlsx
+++ b/ePICreator/data/Humalog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoalmeida/Desktop/hl7Europe/gravitate/gravitate-health/ePICreator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794121DF-8DBF-B446-ADF7-229CBB121CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FD85CB-8FE1-EF4F-83A9-1C7A4C5E9557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" firstSheet="1" activeTab="10" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" firstSheet="1" activeTab="2" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
   </bookViews>
   <sheets>
     <sheet name="AdministrableProductDefinition" sheetId="1" r:id="rId1"/>
@@ -1130,9 +1130,6 @@
   </si>
   <si>
     <t>humalog-id</t>
-  </si>
-  <si>
-    <t>dk</t>
   </si>
   <si>
     <t>&lt;p&gt;B. INDLÆGSSEDDEL 
@@ -1687,6 +1684,9 @@
 - Kontakt lægen eller apotekspersonalet, hvis du får bivirkninger, herunder bivirkninger, som ikke 
 er nævnt i denne indlægsseddel. Se punkt 4.&lt;br /&gt;
 Se den nyeste indlægsseddel på www.indlaegsseddel.dk. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>da</t>
   </si>
 </sst>
 </file>
@@ -1870,9 +1870,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1910,7 +1910,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2016,7 +2016,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2158,7 +2158,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2369,8 +2369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB4B3880-CBCE-B242-93DB-BF401DA7FB8A}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2423,7 +2423,7 @@
         <v>136</v>
       </c>
       <c r="E3" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2497,8 +2497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05DE958-7C5A-B14B-9983-3CEB258B5640}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2613,31 +2613,31 @@
         <v>50</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>180</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>